<commit_message>
Downloading of swaps in Excel format.
</commit_message>
<xml_diff>
--- a/Risk_Aaron/Swap_Symbol_Details.xlsx
+++ b/Risk_Aaron/Swap_Symbol_Details.xlsx
@@ -716,10 +716,10 @@
         </is>
       </c>
       <c r="U4" t="n">
-        <v>-3.2461</v>
+        <v>-3.2329</v>
       </c>
       <c r="V4" t="n">
-        <v>-2.3298</v>
+        <v>-2.3793</v>
       </c>
     </row>
     <row r="5">
@@ -964,10 +964,10 @@
         </is>
       </c>
       <c r="U7" t="n">
-        <v>21.986</v>
+        <v>31.13</v>
       </c>
       <c r="V7" t="n">
-        <v>-46.387</v>
+        <v>-57.728</v>
       </c>
     </row>
     <row r="8">
@@ -1036,10 +1036,10 @@
         </is>
       </c>
       <c r="U8" t="n">
-        <v>-3.6584</v>
+        <v>-3.2294</v>
       </c>
       <c r="V8" t="n">
-        <v>-7.0246</v>
+        <v>-7.4361</v>
       </c>
     </row>
     <row r="9">
@@ -1108,10 +1108,10 @@
         </is>
       </c>
       <c r="U9" t="n">
-        <v>-79.3386</v>
+        <v>-80.2813</v>
       </c>
       <c r="V9" t="n">
-        <v>-157.7411</v>
+        <v>-160.2216</v>
       </c>
     </row>
     <row r="10">
@@ -1180,10 +1180,10 @@
         </is>
       </c>
       <c r="U10" t="n">
-        <v>17.2502</v>
+        <v>19.7708</v>
       </c>
       <c r="V10" t="n">
-        <v>-38.3744</v>
+        <v>-40.9614</v>
       </c>
     </row>
     <row r="11">
@@ -1252,10 +1252,10 @@
         </is>
       </c>
       <c r="U11" t="n">
-        <v>5.5512</v>
+        <v>4.4625</v>
       </c>
       <c r="V11" t="n">
-        <v>-16.8798</v>
+        <v>-15.5193</v>
       </c>
     </row>
     <row r="12">
@@ -1324,10 +1324,10 @@
         </is>
       </c>
       <c r="U12" t="n">
-        <v>139.075</v>
+        <v>224.688</v>
       </c>
       <c r="V12" t="n">
-        <v>-213.719</v>
+        <v>-318.362</v>
       </c>
     </row>
     <row r="13">
@@ -1396,10 +1396,10 @@
         </is>
       </c>
       <c r="U13" t="n">
-        <v>-16.9095</v>
+        <v>-16.9304</v>
       </c>
       <c r="V13" t="n">
-        <v>-25.0782</v>
+        <v>-24.9555</v>
       </c>
     </row>
     <row r="14">
@@ -1468,10 +1468,10 @@
         </is>
       </c>
       <c r="U14" t="n">
-        <v>0.7751</v>
+        <v>0.5618</v>
       </c>
       <c r="V14" t="n">
-        <v>-7.2425</v>
+        <v>-6.9554</v>
       </c>
     </row>
     <row r="15">
@@ -1540,10 +1540,10 @@
         </is>
       </c>
       <c r="U15" t="n">
-        <v>1.5158</v>
+        <v>1.5068</v>
       </c>
       <c r="V15" t="n">
-        <v>-12.8785</v>
+        <v>-12.8775</v>
       </c>
     </row>
     <row r="16">
@@ -1692,10 +1692,10 @@
         </is>
       </c>
       <c r="U17" t="n">
-        <v>-9.832700000000001</v>
+        <v>-7.603</v>
       </c>
       <c r="V17" t="n">
-        <v>-10.7671</v>
+        <v>-13.4897</v>
       </c>
     </row>
     <row r="18">
@@ -1764,10 +1764,10 @@
         </is>
       </c>
       <c r="U18" t="n">
-        <v>-15.3062</v>
+        <v>-17.0972</v>
       </c>
       <c r="V18" t="n">
-        <v>-38.2395</v>
+        <v>-37.4958</v>
       </c>
     </row>
     <row r="19">
@@ -1836,10 +1836,10 @@
         </is>
       </c>
       <c r="U19" t="n">
-        <v>-18.673</v>
+        <v>-14.4655</v>
       </c>
       <c r="V19" t="n">
-        <v>-42.9649</v>
+        <v>-48.4154</v>
       </c>
     </row>
     <row r="20">
@@ -1908,10 +1908,10 @@
         </is>
       </c>
       <c r="U20" t="n">
-        <v>-5.5319</v>
+        <v>-2.01</v>
       </c>
       <c r="V20" t="n">
-        <v>-17.5483</v>
+        <v>-22.935</v>
       </c>
     </row>
     <row r="21">
@@ -1980,10 +1980,10 @@
         </is>
       </c>
       <c r="U21" t="n">
-        <v>-2.1813</v>
+        <v>-1.87</v>
       </c>
       <c r="V21" t="n">
-        <v>0.4644</v>
+        <v>0.3654</v>
       </c>
     </row>
     <row r="22">
@@ -2052,10 +2052,10 @@
         </is>
       </c>
       <c r="U22" t="n">
-        <v>-1.9932</v>
+        <v>-2.1549</v>
       </c>
       <c r="V22" t="n">
-        <v>-1.0362</v>
+        <v>-0.8118</v>
       </c>
     </row>
     <row r="23">
@@ -2124,10 +2124,10 @@
         </is>
       </c>
       <c r="U23" t="n">
-        <v>0.5238</v>
+        <v>0.4536</v>
       </c>
       <c r="V23" t="n">
-        <v>-3.091</v>
+        <v>-2.9612</v>
       </c>
     </row>
     <row r="24">
@@ -2196,10 +2196,10 @@
         </is>
       </c>
       <c r="U24" t="n">
-        <v>-0.7238</v>
+        <v>-0.9031</v>
       </c>
       <c r="V24" t="n">
-        <v>-1.7655</v>
+        <v>-1.5807</v>
       </c>
     </row>
     <row r="25">
@@ -2268,10 +2268,10 @@
         </is>
       </c>
       <c r="U25" t="n">
-        <v>-2.3804</v>
+        <v>-2.442</v>
       </c>
       <c r="V25" t="n">
-        <v>-1.0417</v>
+        <v>-0.9735</v>
       </c>
     </row>
     <row r="26">
@@ -2340,10 +2340,10 @@
         </is>
       </c>
       <c r="U26" t="n">
-        <v>-3.2362</v>
+        <v>-3.3198</v>
       </c>
       <c r="V26" t="n">
-        <v>-1.4377</v>
+        <v>-1.2551</v>
       </c>
     </row>
     <row r="27">
@@ -2412,10 +2412,10 @@
         </is>
       </c>
       <c r="U27" t="n">
-        <v>-2.4365</v>
+        <v>-2.6125</v>
       </c>
       <c r="V27" t="n">
-        <v>-1.9844</v>
+        <v>-1.8117</v>
       </c>
     </row>
     <row r="28">
@@ -2484,10 +2484,10 @@
         </is>
       </c>
       <c r="U28" t="n">
-        <v>0.8289</v>
+        <v>0.837</v>
       </c>
       <c r="V28" t="n">
-        <v>-3.6817</v>
+        <v>-3.6971</v>
       </c>
     </row>
     <row r="29">
@@ -2556,10 +2556,10 @@
         </is>
       </c>
       <c r="U29" t="n">
-        <v>-0.3465</v>
+        <v>-0.3311</v>
       </c>
       <c r="V29" t="n">
-        <v>-2.3067</v>
+        <v>-2.299</v>
       </c>
     </row>
     <row r="30">
@@ -2628,10 +2628,10 @@
         </is>
       </c>
       <c r="U30" t="n">
-        <v>0.0613</v>
+        <v>0.0496</v>
       </c>
       <c r="V30" t="n">
-        <v>-1.7666</v>
+        <v>-1.7589</v>
       </c>
     </row>
     <row r="31">
@@ -2700,10 +2700,10 @@
         </is>
       </c>
       <c r="U31" t="n">
-        <v>-4.4209</v>
+        <v>-4.4539</v>
       </c>
       <c r="V31" t="n">
-        <v>0.5904</v>
+        <v>0.6173999999999999</v>
       </c>
     </row>
     <row r="32">
@@ -2768,10 +2768,10 @@
         </is>
       </c>
       <c r="U32" t="n">
-        <v>-9.924200000000001</v>
+        <v>-9.9</v>
       </c>
       <c r="V32" t="n">
-        <v>-2.7632</v>
+        <v>-2.7588</v>
       </c>
     </row>
     <row r="33">
@@ -2840,10 +2840,10 @@
         </is>
       </c>
       <c r="U33" t="n">
-        <v>-6.0423</v>
+        <v>-5.8729</v>
       </c>
       <c r="V33" t="n">
-        <v>0.4446</v>
+        <v>0.2845</v>
       </c>
     </row>
     <row r="34">
@@ -2912,10 +2912,10 @@
         </is>
       </c>
       <c r="U34" t="n">
-        <v>-6.0467</v>
+        <v>-6.1072</v>
       </c>
       <c r="V34" t="n">
-        <v>0.882</v>
+        <v>0.9324</v>
       </c>
     </row>
     <row r="35">
@@ -2984,10 +2984,10 @@
         </is>
       </c>
       <c r="U35" t="n">
-        <v>-0.8613</v>
+        <v>-0.8756</v>
       </c>
       <c r="V35" t="n">
-        <v>-2.6004</v>
+        <v>-2.574</v>
       </c>
     </row>
     <row r="36">
@@ -3136,7 +3136,7 @@
         </is>
       </c>
       <c r="U37" t="n">
-        <v>-4.0513</v>
+        <v>-4.0447</v>
       </c>
       <c r="V37" t="n">
         <v>-0.3784</v>
@@ -3288,10 +3288,10 @@
         </is>
       </c>
       <c r="U39" t="n">
-        <v>-4.1206</v>
+        <v>-4.2273</v>
       </c>
       <c r="V39" t="n">
-        <v>-0.0528</v>
+        <v>-0.0001</v>
       </c>
     </row>
     <row r="40">
@@ -3520,10 +3520,10 @@
         </is>
       </c>
       <c r="U42" t="n">
-        <v>-7.2501</v>
+        <v>-7.029</v>
       </c>
       <c r="V42" t="n">
-        <v>1.1772</v>
+        <v>1.0467</v>
       </c>
     </row>
     <row r="43">
@@ -3752,10 +3752,10 @@
         </is>
       </c>
       <c r="U45" t="n">
-        <v>-8.2973</v>
+        <v>-8.1972</v>
       </c>
       <c r="V45" t="n">
-        <v>0.3088</v>
+        <v>0.3348</v>
       </c>
     </row>
     <row r="46">
@@ -3904,10 +3904,10 @@
         </is>
       </c>
       <c r="U47" t="n">
-        <v>-5.0327</v>
+        <v>-5.3967</v>
       </c>
       <c r="V47" t="n">
-        <v>0.5805</v>
+        <v>0.5833</v>
       </c>
     </row>
     <row r="48">
@@ -3976,10 +3976,10 @@
         </is>
       </c>
       <c r="U48" t="n">
-        <v>-4.1569</v>
+        <v>-3.8797</v>
       </c>
       <c r="V48" t="n">
-        <v>-4.5892</v>
+        <v>-4.8565</v>
       </c>
     </row>
     <row r="49">
@@ -4048,10 +4048,10 @@
         </is>
       </c>
       <c r="U49" t="n">
-        <v>-4.8829</v>
+        <v>-4.9852</v>
       </c>
       <c r="V49" t="n">
-        <v>-3.4309</v>
+        <v>-3.3242</v>
       </c>
     </row>
     <row r="50">
@@ -4120,10 +4120,10 @@
         </is>
       </c>
       <c r="U50" t="n">
-        <v>0.4023</v>
+        <v>0.3789</v>
       </c>
       <c r="V50" t="n">
-        <v>-6.9278</v>
+        <v>-6.8959</v>
       </c>
     </row>
     <row r="51">
@@ -4272,10 +4272,10 @@
         </is>
       </c>
       <c r="U52" t="n">
-        <v>-2.3958</v>
+        <v>-2.4926</v>
       </c>
       <c r="V52" t="n">
-        <v>-4.6222</v>
+        <v>-4.5177</v>
       </c>
     </row>
     <row r="53">
@@ -4424,10 +4424,10 @@
         </is>
       </c>
       <c r="U54" t="n">
-        <v>-6.402</v>
+        <v>-6.162</v>
       </c>
       <c r="V54" t="n">
-        <v>-4.056</v>
+        <v>-4.3116</v>
       </c>
     </row>
     <row r="55">
@@ -4576,10 +4576,10 @@
         </is>
       </c>
       <c r="U56" t="n">
-        <v>-5.5528</v>
+        <v>-5.4868</v>
       </c>
       <c r="V56" t="n">
-        <v>-2.8072</v>
+        <v>-2.6708</v>
       </c>
     </row>
     <row r="57">
@@ -4648,10 +4648,10 @@
         </is>
       </c>
       <c r="U57" t="n">
-        <v>-3.6938</v>
+        <v>-3.8808</v>
       </c>
       <c r="V57" t="n">
-        <v>-3.0943</v>
+        <v>-3.0316</v>
       </c>
     </row>
     <row r="58">
@@ -5040,10 +5040,10 @@
         </is>
       </c>
       <c r="U62" t="n">
-        <v>-1.188</v>
+        <v>-1.3464</v>
       </c>
       <c r="V62" t="n">
-        <v>-1.5477</v>
+        <v>-1.3519</v>
       </c>
     </row>
     <row r="63">
@@ -5112,10 +5112,10 @@
         </is>
       </c>
       <c r="U63" t="n">
-        <v>0.7371</v>
+        <v>0.6912</v>
       </c>
       <c r="V63" t="n">
-        <v>-3.3418</v>
+        <v>-3.2351</v>
       </c>
     </row>
     <row r="64">
@@ -5184,10 +5184,10 @@
         </is>
       </c>
       <c r="U64" t="n">
-        <v>-0.1848</v>
+        <v>-0.3113</v>
       </c>
       <c r="V64" t="n">
-        <v>-2.1076</v>
+        <v>-1.9767</v>
       </c>
     </row>
     <row r="65">
@@ -5256,10 +5256,10 @@
         </is>
       </c>
       <c r="U65" t="n">
-        <v>-2.3793</v>
+        <v>-2.4409</v>
       </c>
       <c r="V65" t="n">
-        <v>-2.0603</v>
+        <v>-1.87</v>
       </c>
     </row>
     <row r="66">
@@ -6048,10 +6048,10 @@
         </is>
       </c>
       <c r="U75" t="n">
-        <v>-1.3402</v>
+        <v>-1.3686</v>
       </c>
       <c r="V75" t="n">
-        <v>-3.4171</v>
+        <v>-3.5619</v>
       </c>
     </row>
     <row r="76">

</xml_diff>

<commit_message>
Updated Swap excel print outs
</commit_message>
<xml_diff>
--- a/Risk_Aaron/Swap_Symbol_Details.xlsx
+++ b/Risk_Aaron/Swap_Symbol_Details.xlsx
@@ -716,10 +716,10 @@
         </is>
       </c>
       <c r="U4" t="n">
-        <v>-3.3011</v>
+        <v>-3.345</v>
       </c>
       <c r="V4" t="n">
-        <v>-2.2143</v>
+        <v>-2.169</v>
       </c>
     </row>
     <row r="5">
@@ -964,10 +964,10 @@
         </is>
       </c>
       <c r="U7" t="n">
-        <v>28.678</v>
+        <v>27.6091</v>
       </c>
       <c r="V7" t="n">
-        <v>-54.637</v>
+        <v>-53.17</v>
       </c>
     </row>
     <row r="8">
@@ -1036,10 +1036,10 @@
         </is>
       </c>
       <c r="U8" t="n">
-        <v>-3.3264</v>
+        <v>-3.5076</v>
       </c>
       <c r="V8" t="n">
-        <v>-7.3364</v>
+        <v>-7.1422</v>
       </c>
     </row>
     <row r="9">
@@ -1108,10 +1108,10 @@
         </is>
       </c>
       <c r="U9" t="n">
-        <v>-79.1604</v>
+        <v>-78.70699999999999</v>
       </c>
       <c r="V9" t="n">
-        <v>-158.1701</v>
+        <v>-157.271</v>
       </c>
     </row>
     <row r="10">
@@ -1180,10 +1180,10 @@
         </is>
       </c>
       <c r="U10" t="n">
-        <v>45.4267</v>
+        <v>41.1387</v>
       </c>
       <c r="V10" t="n">
-        <v>-72.2543</v>
+        <v>-66.9823</v>
       </c>
     </row>
     <row r="11">
@@ -1252,10 +1252,10 @@
         </is>
       </c>
       <c r="U11" t="n">
-        <v>-2.0845</v>
+        <v>-2.1749</v>
       </c>
       <c r="V11" t="n">
-        <v>-7.5668</v>
+        <v>-7.4385</v>
       </c>
     </row>
     <row r="12">
@@ -1324,10 +1324,10 @@
         </is>
       </c>
       <c r="U12" t="n">
-        <v>218.839</v>
+        <v>197.0945</v>
       </c>
       <c r="V12" t="n">
-        <v>-311.454</v>
+        <v>-284.81</v>
       </c>
     </row>
     <row r="13">
@@ -1396,10 +1396,10 @@
         </is>
       </c>
       <c r="U13" t="n">
-        <v>-16.8813</v>
+        <v>-17.0854</v>
       </c>
       <c r="V13" t="n">
-        <v>-24.8688</v>
+        <v>-24.5093</v>
       </c>
     </row>
     <row r="14">
@@ -1468,10 +1468,10 @@
         </is>
       </c>
       <c r="U14" t="n">
-        <v>0.2627</v>
+        <v>0.06419999999999999</v>
       </c>
       <c r="V14" t="n">
-        <v>-6.5792</v>
+        <v>-6.3302</v>
       </c>
     </row>
     <row r="15">
@@ -1540,10 +1540,10 @@
         </is>
       </c>
       <c r="U15" t="n">
-        <v>0.6279</v>
+        <v>0.1029</v>
       </c>
       <c r="V15" t="n">
-        <v>-11.817</v>
+        <v>-11.1824</v>
       </c>
     </row>
     <row r="16">
@@ -1692,10 +1692,10 @@
         </is>
       </c>
       <c r="U17" t="n">
-        <v>-7.5262</v>
+        <v>-7.8636</v>
       </c>
       <c r="V17" t="n">
-        <v>-13.7142</v>
+        <v>-13.3782</v>
       </c>
     </row>
     <row r="18">
@@ -1764,10 +1764,10 @@
         </is>
       </c>
       <c r="U18" t="n">
-        <v>-13.0074</v>
+        <v>-14.3895</v>
       </c>
       <c r="V18" t="n">
-        <v>-42.1028</v>
+        <v>-40.5616</v>
       </c>
     </row>
     <row r="19">
@@ -1836,10 +1836,10 @@
         </is>
       </c>
       <c r="U19" t="n">
-        <v>-11.1615</v>
+        <v>-13.1448</v>
       </c>
       <c r="V19" t="n">
-        <v>-52.8077</v>
+        <v>-50.679</v>
       </c>
     </row>
     <row r="20">
@@ -1908,10 +1908,10 @@
         </is>
       </c>
       <c r="U20" t="n">
-        <v>0.3258</v>
+        <v>0.7593</v>
       </c>
       <c r="V20" t="n">
-        <v>-23.0483</v>
+        <v>-22.991</v>
       </c>
     </row>
     <row r="21">
@@ -1980,10 +1980,10 @@
         </is>
       </c>
       <c r="U21" t="n">
-        <v>-1.9217</v>
+        <v>-1.921</v>
       </c>
       <c r="V21" t="n">
-        <v>0.3762</v>
+        <v>0.3755</v>
       </c>
     </row>
     <row r="22">
@@ -2052,10 +2052,10 @@
         </is>
       </c>
       <c r="U22" t="n">
-        <v>-2.2781</v>
+        <v>-2.301</v>
       </c>
       <c r="V22" t="n">
-        <v>-0.638</v>
+        <v>-0.613</v>
       </c>
     </row>
     <row r="23">
@@ -2124,10 +2124,10 @@
         </is>
       </c>
       <c r="U23" t="n">
-        <v>0.3942</v>
+        <v>0.3829</v>
       </c>
       <c r="V23" t="n">
-        <v>-2.8468</v>
+        <v>-2.827</v>
       </c>
     </row>
     <row r="24">
@@ -2196,10 +2196,10 @@
         </is>
       </c>
       <c r="U24" t="n">
-        <v>-1.0769</v>
+        <v>-1.112</v>
       </c>
       <c r="V24" t="n">
-        <v>-1.4003</v>
+        <v>-1.366</v>
       </c>
     </row>
     <row r="25">
@@ -2268,10 +2268,10 @@
         </is>
       </c>
       <c r="U25" t="n">
-        <v>-2.4772</v>
+        <v>-2.464</v>
       </c>
       <c r="V25" t="n">
-        <v>-0.9273</v>
+        <v>-0.9350000000000001</v>
       </c>
     </row>
     <row r="26">
@@ -2340,10 +2340,10 @@
         </is>
       </c>
       <c r="U26" t="n">
-        <v>-3.2802</v>
+        <v>-3.281</v>
       </c>
       <c r="V26" t="n">
-        <v>-1.1759</v>
+        <v>-1.161</v>
       </c>
     </row>
     <row r="27">
@@ -2412,10 +2412,10 @@
         </is>
       </c>
       <c r="U27" t="n">
-        <v>-2.7357</v>
+        <v>-2.755</v>
       </c>
       <c r="V27" t="n">
-        <v>-1.6863</v>
+        <v>-1.666</v>
       </c>
     </row>
     <row r="28">
@@ -2487,7 +2487,7 @@
         <v>0.837</v>
       </c>
       <c r="V28" t="n">
-        <v>-3.6971</v>
+        <v>-3.696</v>
       </c>
     </row>
     <row r="29">
@@ -2556,10 +2556,10 @@
         </is>
       </c>
       <c r="U29" t="n">
-        <v>-0.3487</v>
+        <v>-0.362</v>
       </c>
       <c r="V29" t="n">
-        <v>-2.2616</v>
+        <v>-2.248</v>
       </c>
     </row>
     <row r="30">
@@ -2628,10 +2628,10 @@
         </is>
       </c>
       <c r="U30" t="n">
-        <v>0.0451</v>
+        <v>0.0459</v>
       </c>
       <c r="V30" t="n">
-        <v>-1.6962</v>
+        <v>-1.686</v>
       </c>
     </row>
     <row r="31">
@@ -2700,10 +2700,10 @@
         </is>
       </c>
       <c r="U31" t="n">
-        <v>-4.5089</v>
+        <v>-4.522</v>
       </c>
       <c r="V31" t="n">
-        <v>0.6606</v>
+        <v>0.6693</v>
       </c>
     </row>
     <row r="32">
@@ -2768,10 +2768,10 @@
         </is>
       </c>
       <c r="U32" t="n">
-        <v>-9.8912</v>
+        <v>-9.890000000000001</v>
       </c>
       <c r="V32" t="n">
-        <v>-2.7566</v>
+        <v>-2.756</v>
       </c>
     </row>
     <row r="33">
@@ -2840,10 +2840,10 @@
         </is>
       </c>
       <c r="U33" t="n">
-        <v>-5.5055</v>
+        <v>-5.429</v>
       </c>
       <c r="V33" t="n">
-        <v>0.1549</v>
+        <v>0.1318</v>
       </c>
     </row>
     <row r="34">
@@ -2912,10 +2912,10 @@
         </is>
       </c>
       <c r="U34" t="n">
-        <v>-6.1314</v>
+        <v>-6.135</v>
       </c>
       <c r="V34" t="n">
-        <v>0.963</v>
+        <v>0.9671</v>
       </c>
     </row>
     <row r="35">
@@ -2984,10 +2984,10 @@
         </is>
       </c>
       <c r="U35" t="n">
-        <v>-0.8734</v>
+        <v>-0.875</v>
       </c>
       <c r="V35" t="n">
-        <v>-2.5674</v>
+        <v>-2.567</v>
       </c>
     </row>
     <row r="36">
@@ -3136,10 +3136,10 @@
         </is>
       </c>
       <c r="U37" t="n">
-        <v>-4.0579</v>
+        <v>-4.063</v>
       </c>
       <c r="V37" t="n">
-        <v>-0.3608</v>
+        <v>-0.356</v>
       </c>
     </row>
     <row r="38">
@@ -3288,10 +3288,10 @@
         </is>
       </c>
       <c r="U39" t="n">
-        <v>-4.2229</v>
+        <v>-4.217</v>
       </c>
       <c r="V39" t="n">
-        <v>0.0575</v>
+        <v>0.06950000000000001</v>
       </c>
     </row>
     <row r="40">
@@ -3520,10 +3520,10 @@
         </is>
       </c>
       <c r="U42" t="n">
-        <v>-6.809</v>
+        <v>-6.749</v>
       </c>
       <c r="V42" t="n">
-        <v>0.9153</v>
+        <v>0.8787</v>
       </c>
     </row>
     <row r="43">
@@ -3752,10 +3752,10 @@
         </is>
       </c>
       <c r="U45" t="n">
-        <v>-7.9222</v>
+        <v>-7.885</v>
       </c>
       <c r="V45" t="n">
-        <v>0.2898</v>
+        <v>0.2823</v>
       </c>
     </row>
     <row r="46">
@@ -3904,10 +3904,10 @@
         </is>
       </c>
       <c r="U47" t="n">
-        <v>-5.5165</v>
+        <v>-5.5245</v>
       </c>
       <c r="V47" t="n">
-        <v>0.5810999999999999</v>
+        <v>0.5821</v>
       </c>
     </row>
     <row r="48">
@@ -3976,10 +3976,10 @@
         </is>
       </c>
       <c r="U48" t="n">
-        <v>-3.5739</v>
+        <v>-3.518</v>
       </c>
       <c r="V48" t="n">
-        <v>-5.1403</v>
+        <v>-5.194</v>
       </c>
     </row>
     <row r="49">
@@ -4048,10 +4048,10 @@
         </is>
       </c>
       <c r="U49" t="n">
-        <v>-4.9588</v>
+        <v>-4.938</v>
       </c>
       <c r="V49" t="n">
-        <v>-3.3374</v>
+        <v>-3.355</v>
       </c>
     </row>
     <row r="50">
@@ -4120,10 +4120,10 @@
         </is>
       </c>
       <c r="U50" t="n">
-        <v>0.3753</v>
+        <v>0.3764</v>
       </c>
       <c r="V50" t="n">
-        <v>-6.8959</v>
+        <v>-6.898</v>
       </c>
     </row>
     <row r="51">
@@ -4272,10 +4272,10 @@
         </is>
       </c>
       <c r="U52" t="n">
-        <v>-2.5564</v>
+        <v>-2.572</v>
       </c>
       <c r="V52" t="n">
-        <v>-4.4407</v>
+        <v>-4.423</v>
       </c>
     </row>
     <row r="53">
@@ -4424,10 +4424,10 @@
         </is>
       </c>
       <c r="U54" t="n">
-        <v>-5.8596</v>
+        <v>-5.7676</v>
       </c>
       <c r="V54" t="n">
-        <v>-4.614</v>
+        <v>-4.7051</v>
       </c>
     </row>
     <row r="55">
@@ -4576,10 +4576,10 @@
         </is>
       </c>
       <c r="U56" t="n">
-        <v>-5.225</v>
+        <v>-5.197</v>
       </c>
       <c r="V56" t="n">
-        <v>-2.9414</v>
+        <v>-3.017</v>
       </c>
     </row>
     <row r="57">
@@ -4648,10 +4648,10 @@
         </is>
       </c>
       <c r="U57" t="n">
-        <v>-3.8852</v>
+        <v>-3.881</v>
       </c>
       <c r="V57" t="n">
-        <v>-3.0228</v>
+        <v>-3.026</v>
       </c>
     </row>
     <row r="58">
@@ -5040,10 +5040,10 @@
         </is>
       </c>
       <c r="U62" t="n">
-        <v>-1.4674</v>
+        <v>-1.496</v>
       </c>
       <c r="V62" t="n">
-        <v>-1.1957</v>
+        <v>-1.169</v>
       </c>
     </row>
     <row r="63">
@@ -5112,10 +5112,10 @@
         </is>
       </c>
       <c r="U63" t="n">
-        <v>0.6516</v>
+        <v>0.6382</v>
       </c>
       <c r="V63" t="n">
-        <v>-3.1317</v>
+        <v>-3.108</v>
       </c>
     </row>
     <row r="64">
@@ -5184,10 +5184,10 @@
         </is>
       </c>
       <c r="U64" t="n">
-        <v>-0.4301</v>
+        <v>-0.466</v>
       </c>
       <c r="V64" t="n">
-        <v>-1.8447</v>
+        <v>-1.806</v>
       </c>
     </row>
     <row r="65">
@@ -5256,10 +5256,10 @@
         </is>
       </c>
       <c r="U65" t="n">
-        <v>-2.3903</v>
+        <v>-2.4</v>
       </c>
       <c r="V65" t="n">
-        <v>-1.826</v>
+        <v>-1.816</v>
       </c>
     </row>
     <row r="66">
@@ -6048,10 +6048,10 @@
         </is>
       </c>
       <c r="U75" t="n">
-        <v>-1.4442</v>
+        <v>-1.4613</v>
       </c>
       <c r="V75" t="n">
-        <v>-3.5729</v>
+        <v>-3.5601</v>
       </c>
     </row>
     <row r="76">

</xml_diff>

<commit_message>
Swaps upload. Identifying Fixed swaps as well as Bloomberg dividend
</commit_message>
<xml_diff>
--- a/Risk_Aaron/Swap_Symbol_Details.xlsx
+++ b/Risk_Aaron/Swap_Symbol_Details.xlsx
@@ -716,10 +716,10 @@
         </is>
       </c>
       <c r="U4" t="n">
-        <v>-3.415</v>
+        <v>-3.5706</v>
       </c>
       <c r="V4" t="n">
-        <v>-2.072</v>
+        <v>-1.9448</v>
       </c>
     </row>
     <row r="5">
@@ -964,10 +964,10 @@
         </is>
       </c>
       <c r="U7" t="n">
-        <v>67.30549999999999</v>
+        <v>64.495</v>
       </c>
       <c r="V7" t="n">
-        <v>-101.44</v>
+        <v>-98.164</v>
       </c>
     </row>
     <row r="8">
@@ -1036,10 +1036,10 @@
         </is>
       </c>
       <c r="U8" t="n">
-        <v>-3.5096</v>
+        <v>-4.3963</v>
       </c>
       <c r="V8" t="n">
-        <v>-7.1434</v>
+        <v>-6.1616</v>
       </c>
     </row>
     <row r="9">
@@ -1108,10 +1108,10 @@
         </is>
       </c>
       <c r="U9" t="n">
-        <v>-78.206</v>
+        <v>-77.5291</v>
       </c>
       <c r="V9" t="n">
-        <v>-156.348</v>
+        <v>-154.9163</v>
       </c>
     </row>
     <row r="10">
@@ -1180,10 +1180,10 @@
         </is>
       </c>
       <c r="U10" t="n">
-        <v>41.1592</v>
+        <v>30.1014</v>
       </c>
       <c r="V10" t="n">
-        <v>-66.94929999999999</v>
+        <v>-53.5347</v>
       </c>
     </row>
     <row r="11">
@@ -1252,10 +1252,10 @@
         </is>
       </c>
       <c r="U11" t="n">
-        <v>-2.1692</v>
+        <v>-2.0678</v>
       </c>
       <c r="V11" t="n">
-        <v>-7.4302</v>
+        <v>-7.5332</v>
       </c>
     </row>
     <row r="12">
@@ -1324,10 +1324,10 @@
         </is>
       </c>
       <c r="U12" t="n">
-        <v>69.1409</v>
+        <v>77.551</v>
       </c>
       <c r="V12" t="n">
-        <v>-128.66</v>
+        <v>-138.6</v>
       </c>
     </row>
     <row r="13">
@@ -1396,10 +1396,10 @@
         </is>
       </c>
       <c r="U13" t="n">
-        <v>-17.036</v>
+        <v>-19.8042</v>
       </c>
       <c r="V13" t="n">
-        <v>-24.4816</v>
+        <v>-21.395</v>
       </c>
     </row>
     <row r="14">
@@ -1468,10 +1468,10 @@
         </is>
       </c>
       <c r="U14" t="n">
-        <v>0.0674</v>
+        <v>0.2718</v>
       </c>
       <c r="V14" t="n">
-        <v>-6.3258</v>
+        <v>-6.5608</v>
       </c>
     </row>
     <row r="15">
@@ -1540,10 +1540,10 @@
         </is>
       </c>
       <c r="U15" t="n">
-        <v>0.1038</v>
+        <v>0.6367</v>
       </c>
       <c r="V15" t="n">
-        <v>-11.1817</v>
+        <v>-11.812</v>
       </c>
     </row>
     <row r="16">
@@ -1692,10 +1692,10 @@
         </is>
       </c>
       <c r="U17" t="n">
-        <v>-7.8973</v>
+        <v>-7.9873</v>
       </c>
       <c r="V17" t="n">
-        <v>-13.4031</v>
+        <v>-13.4267</v>
       </c>
     </row>
     <row r="18">
@@ -1764,10 +1764,10 @@
         </is>
       </c>
       <c r="U18" t="n">
-        <v>-14.4394</v>
+        <v>-13.1026</v>
       </c>
       <c r="V18" t="n">
-        <v>-40.5927</v>
+        <v>-42.1853</v>
       </c>
     </row>
     <row r="19">
@@ -1836,10 +1836,10 @@
         </is>
       </c>
       <c r="U19" t="n">
-        <v>-13.1308</v>
+        <v>-7.6658</v>
       </c>
       <c r="V19" t="n">
-        <v>-50.821</v>
+        <v>-57.0889</v>
       </c>
     </row>
     <row r="20">
@@ -1908,10 +1908,10 @@
         </is>
       </c>
       <c r="U20" t="n">
-        <v>1.6297</v>
+        <v>2.9878</v>
       </c>
       <c r="V20" t="n">
-        <v>-22.985</v>
+        <v>-23.012</v>
       </c>
     </row>
     <row r="21">
@@ -1980,10 +1980,10 @@
         </is>
       </c>
       <c r="U21" t="n">
-        <v>-1.939</v>
+        <v>-1.958</v>
       </c>
       <c r="V21" t="n">
-        <v>0.3796</v>
+        <v>0.3834</v>
       </c>
     </row>
     <row r="22">
@@ -2052,10 +2052,10 @@
         </is>
       </c>
       <c r="U22" t="n">
-        <v>-2.314</v>
+        <v>-2.3287</v>
       </c>
       <c r="V22" t="n">
-        <v>-0.59</v>
+        <v>-0.5929</v>
       </c>
     </row>
     <row r="23">
@@ -2124,10 +2124,10 @@
         </is>
       </c>
       <c r="U23" t="n">
-        <v>0.369</v>
+        <v>0.3519</v>
       </c>
       <c r="V23" t="n">
-        <v>-2.804</v>
+        <v>-2.783</v>
       </c>
     </row>
     <row r="24">
@@ -2196,10 +2196,10 @@
         </is>
       </c>
       <c r="U24" t="n">
-        <v>-1.124</v>
+        <v>-1.1374</v>
       </c>
       <c r="V24" t="n">
-        <v>-1.349</v>
+        <v>-1.3365</v>
       </c>
     </row>
     <row r="25">
@@ -2268,10 +2268,10 @@
         </is>
       </c>
       <c r="U25" t="n">
-        <v>-2.431</v>
+        <v>-2.3298</v>
       </c>
       <c r="V25" t="n">
-        <v>-0.962</v>
+        <v>-1.045</v>
       </c>
     </row>
     <row r="26">
@@ -2340,10 +2340,10 @@
         </is>
       </c>
       <c r="U26" t="n">
-        <v>-3.255</v>
+        <v>-3.2604</v>
       </c>
       <c r="V26" t="n">
-        <v>-1.148</v>
+        <v>-1.1363</v>
       </c>
     </row>
     <row r="27">
@@ -2412,10 +2412,10 @@
         </is>
       </c>
       <c r="U27" t="n">
-        <v>-2.786</v>
+        <v>-2.8105</v>
       </c>
       <c r="V27" t="n">
-        <v>-1.635</v>
+        <v>-1.6082</v>
       </c>
     </row>
     <row r="28">
@@ -2484,10 +2484,10 @@
         </is>
       </c>
       <c r="U28" t="n">
-        <v>0.8296</v>
+        <v>0.819</v>
       </c>
       <c r="V28" t="n">
-        <v>-3.684</v>
+        <v>-3.6641</v>
       </c>
     </row>
     <row r="29">
@@ -2556,10 +2556,10 @@
         </is>
       </c>
       <c r="U29" t="n">
-        <v>-0.348</v>
+        <v>-0.3597</v>
       </c>
       <c r="V29" t="n">
-        <v>-2.252</v>
+        <v>-2.2407</v>
       </c>
     </row>
     <row r="30">
@@ -2628,10 +2628,10 @@
         </is>
       </c>
       <c r="U30" t="n">
-        <v>0.0385</v>
+        <v>0.0477</v>
       </c>
       <c r="V30" t="n">
-        <v>-1.687</v>
+        <v>-1.6698</v>
       </c>
     </row>
     <row r="31">
@@ -2700,10 +2700,10 @@
         </is>
       </c>
       <c r="U31" t="n">
-        <v>-4.506</v>
+        <v>-4.4858</v>
       </c>
       <c r="V31" t="n">
-        <v>0.6644</v>
+        <v>0.6534</v>
       </c>
     </row>
     <row r="32">
@@ -2768,10 +2768,10 @@
         </is>
       </c>
       <c r="U32" t="n">
-        <v>-9.898</v>
+        <v>-9.906599999999999</v>
       </c>
       <c r="V32" t="n">
-        <v>-2.758</v>
+        <v>-2.7599</v>
       </c>
     </row>
     <row r="33">
@@ -2840,10 +2840,10 @@
         </is>
       </c>
       <c r="U33" t="n">
-        <v>-5.33</v>
+        <v>-5.225</v>
       </c>
       <c r="V33" t="n">
-        <v>0.1179</v>
+        <v>0.1117</v>
       </c>
     </row>
     <row r="34">
@@ -2912,10 +2912,10 @@
         </is>
       </c>
       <c r="U34" t="n">
-        <v>-6.135</v>
+        <v>-6.1325</v>
       </c>
       <c r="V34" t="n">
-        <v>0.9745</v>
+        <v>0.9765</v>
       </c>
     </row>
     <row r="35">
@@ -2984,10 +2984,10 @@
         </is>
       </c>
       <c r="U35" t="n">
-        <v>-0.878</v>
+        <v>-0.8943</v>
       </c>
       <c r="V35" t="n">
-        <v>-2.562</v>
+        <v>-2.5531</v>
       </c>
     </row>
     <row r="36">
@@ -3136,10 +3136,10 @@
         </is>
       </c>
       <c r="U37" t="n">
-        <v>-4.066</v>
+        <v>-4.0777</v>
       </c>
       <c r="V37" t="n">
-        <v>-0.349</v>
+        <v>-0.3366</v>
       </c>
     </row>
     <row r="38">
@@ -3288,10 +3288,10 @@
         </is>
       </c>
       <c r="U39" t="n">
-        <v>-4.171</v>
+        <v>-4.1151</v>
       </c>
       <c r="V39" t="n">
-        <v>0.0615</v>
+        <v>0.0511</v>
       </c>
     </row>
     <row r="40">
@@ -3520,10 +3520,10 @@
         </is>
       </c>
       <c r="U42" t="n">
-        <v>-6.65</v>
+        <v>-6.4878</v>
       </c>
       <c r="V42" t="n">
-        <v>0.8231000000000001</v>
+        <v>0.7272</v>
       </c>
     </row>
     <row r="43">
@@ -3752,10 +3752,10 @@
         </is>
       </c>
       <c r="U45" t="n">
-        <v>-7.805</v>
+        <v>-7.7869</v>
       </c>
       <c r="V45" t="n">
-        <v>0.2757</v>
+        <v>0.2745</v>
       </c>
     </row>
     <row r="46">
@@ -3904,10 +3904,10 @@
         </is>
       </c>
       <c r="U47" t="n">
-        <v>-5.5887</v>
+        <v>-5.6172</v>
       </c>
       <c r="V47" t="n">
-        <v>0.5855</v>
+        <v>0.5976</v>
       </c>
     </row>
     <row r="48">
@@ -3976,10 +3976,10 @@
         </is>
       </c>
       <c r="U48" t="n">
-        <v>-3.47</v>
+        <v>-3.432</v>
       </c>
       <c r="V48" t="n">
-        <v>-5.242</v>
+        <v>-5.291</v>
       </c>
     </row>
     <row r="49">
@@ -4048,10 +4048,10 @@
         </is>
       </c>
       <c r="U49" t="n">
-        <v>-4.926</v>
+        <v>-4.8686</v>
       </c>
       <c r="V49" t="n">
-        <v>-3.364</v>
+        <v>-3.4144</v>
       </c>
     </row>
     <row r="50">
@@ -4120,10 +4120,10 @@
         </is>
       </c>
       <c r="U50" t="n">
-        <v>0.3698</v>
+        <v>0.3645</v>
       </c>
       <c r="V50" t="n">
-        <v>-6.895</v>
+        <v>-6.8937</v>
       </c>
     </row>
     <row r="51">
@@ -4272,10 +4272,10 @@
         </is>
       </c>
       <c r="U52" t="n">
-        <v>-2.555</v>
+        <v>-2.5421</v>
       </c>
       <c r="V52" t="n">
-        <v>-4.437</v>
+        <v>-4.4506</v>
       </c>
     </row>
     <row r="53">
@@ -4424,10 +4424,10 @@
         </is>
       </c>
       <c r="U54" t="n">
-        <v>-5.6411</v>
+        <v>-5.3988</v>
       </c>
       <c r="V54" t="n">
-        <v>-4.8305</v>
+        <v>-5.07</v>
       </c>
     </row>
     <row r="55">
@@ -4576,10 +4576,10 @@
         </is>
       </c>
       <c r="U56" t="n">
-        <v>-5.09</v>
+        <v>-5.0479</v>
       </c>
       <c r="V56" t="n">
-        <v>-3.025</v>
+        <v>-3.0767</v>
       </c>
     </row>
     <row r="57">
@@ -4648,10 +4648,10 @@
         </is>
       </c>
       <c r="U57" t="n">
-        <v>-3.896</v>
+        <v>-3.9072</v>
       </c>
       <c r="V57" t="n">
-        <v>-3.011</v>
+        <v>-3.0008</v>
       </c>
     </row>
     <row r="58">
@@ -5040,10 +5040,10 @@
         </is>
       </c>
       <c r="U62" t="n">
-        <v>-1.553</v>
+        <v>-1.6357</v>
       </c>
       <c r="V62" t="n">
-        <v>-1.1</v>
+        <v>-1.034</v>
       </c>
     </row>
     <row r="63">
@@ -5112,10 +5112,10 @@
         </is>
       </c>
       <c r="U63" t="n">
-        <v>0.6136</v>
+        <v>0.5652</v>
       </c>
       <c r="V63" t="n">
-        <v>-3.056</v>
+        <v>-2.9832</v>
       </c>
     </row>
     <row r="64">
@@ -5184,10 +5184,10 @@
         </is>
       </c>
       <c r="U64" t="n">
-        <v>-0.5</v>
+        <v>-0.5775</v>
       </c>
       <c r="V64" t="n">
-        <v>-1.764</v>
+        <v>-1.6775</v>
       </c>
     </row>
     <row r="65">
@@ -5256,10 +5256,10 @@
         </is>
       </c>
       <c r="U65" t="n">
-        <v>-2.404</v>
+        <v>-2.4816</v>
       </c>
       <c r="V65" t="n">
-        <v>-1.748</v>
+        <v>-1.6522</v>
       </c>
     </row>
     <row r="66">
@@ -6048,10 +6048,10 @@
         </is>
       </c>
       <c r="U75" t="n">
-        <v>-1.4444</v>
+        <v>-1.4196</v>
       </c>
       <c r="V75" t="n">
-        <v>-3.6175</v>
+        <v>-3.6456</v>
       </c>
     </row>
     <row r="76">

</xml_diff>

<commit_message>
Added Regression for the CFD Swap Models.
</commit_message>
<xml_diff>
--- a/Risk_Aaron/Swap_Symbol_Details.xlsx
+++ b/Risk_Aaron/Swap_Symbol_Details.xlsx
@@ -716,10 +716,10 @@
         </is>
       </c>
       <c r="U4" t="n">
-        <v>-3.5706</v>
+        <v>-3.736</v>
       </c>
       <c r="V4" t="n">
-        <v>-1.9448</v>
+        <v>-1.817</v>
       </c>
     </row>
     <row r="5">
@@ -964,10 +964,10 @@
         </is>
       </c>
       <c r="U7" t="n">
-        <v>64.495</v>
+        <v>70.7473</v>
       </c>
       <c r="V7" t="n">
-        <v>-98.164</v>
+        <v>-105.4</v>
       </c>
     </row>
     <row r="8">
@@ -1036,10 +1036,10 @@
         </is>
       </c>
       <c r="U8" t="n">
-        <v>-4.3963</v>
+        <v>-4.8321</v>
       </c>
       <c r="V8" t="n">
-        <v>-6.1616</v>
+        <v>-5.7309</v>
       </c>
     </row>
     <row r="9">
@@ -1108,10 +1108,10 @@
         </is>
       </c>
       <c r="U9" t="n">
-        <v>-77.5291</v>
+        <v>-77.005</v>
       </c>
       <c r="V9" t="n">
-        <v>-154.9163</v>
+        <v>-153.582</v>
       </c>
     </row>
     <row r="10">
@@ -1180,10 +1180,10 @@
         </is>
       </c>
       <c r="U10" t="n">
-        <v>30.1014</v>
+        <v>26.818</v>
       </c>
       <c r="V10" t="n">
-        <v>-53.5347</v>
+        <v>-49.5337</v>
       </c>
     </row>
     <row r="11">
@@ -1252,10 +1252,10 @@
         </is>
       </c>
       <c r="U11" t="n">
-        <v>-2.0678</v>
+        <v>-2.1697</v>
       </c>
       <c r="V11" t="n">
-        <v>-7.5332</v>
+        <v>-7.4158</v>
       </c>
     </row>
     <row r="12">
@@ -1324,10 +1324,10 @@
         </is>
       </c>
       <c r="U12" t="n">
-        <v>77.551</v>
+        <v>68.7209</v>
       </c>
       <c r="V12" t="n">
-        <v>-138.6</v>
+        <v>-127.65</v>
       </c>
     </row>
     <row r="13">
@@ -1396,10 +1396,10 @@
         </is>
       </c>
       <c r="U13" t="n">
-        <v>-19.8042</v>
+        <v>-19.7602</v>
       </c>
       <c r="V13" t="n">
-        <v>-21.395</v>
+        <v>-21.3967</v>
       </c>
     </row>
     <row r="14">
@@ -1468,10 +1468,10 @@
         </is>
       </c>
       <c r="U14" t="n">
-        <v>0.2718</v>
+        <v>0.0663</v>
       </c>
       <c r="V14" t="n">
-        <v>-6.5608</v>
+        <v>-6.3182</v>
       </c>
     </row>
     <row r="15">
@@ -1540,10 +1540,10 @@
         </is>
       </c>
       <c r="U15" t="n">
-        <v>0.6367</v>
+        <v>-1.177</v>
       </c>
       <c r="V15" t="n">
-        <v>-11.812</v>
+        <v>-9.7224</v>
       </c>
     </row>
     <row r="16">
@@ -1692,10 +1692,10 @@
         </is>
       </c>
       <c r="U17" t="n">
-        <v>-7.9873</v>
+        <v>-8.3057</v>
       </c>
       <c r="V17" t="n">
-        <v>-13.4267</v>
+        <v>-13.1546</v>
       </c>
     </row>
     <row r="18">
@@ -1764,10 +1764,10 @@
         </is>
       </c>
       <c r="U18" t="n">
-        <v>-13.1026</v>
+        <v>-17.3165</v>
       </c>
       <c r="V18" t="n">
-        <v>-42.1853</v>
+        <v>-37.9019</v>
       </c>
     </row>
     <row r="19">
@@ -1836,10 +1836,10 @@
         </is>
       </c>
       <c r="U19" t="n">
-        <v>-7.6658</v>
+        <v>-11.2989</v>
       </c>
       <c r="V19" t="n">
-        <v>-57.0889</v>
+        <v>-53.408</v>
       </c>
     </row>
     <row r="20">
@@ -1908,10 +1908,10 @@
         </is>
       </c>
       <c r="U20" t="n">
-        <v>2.9878</v>
+        <v>3.8551</v>
       </c>
       <c r="V20" t="n">
-        <v>-23.012</v>
+        <v>-23.077</v>
       </c>
     </row>
     <row r="21">
@@ -1980,10 +1980,10 @@
         </is>
       </c>
       <c r="U21" t="n">
-        <v>-1.958</v>
+        <v>-1.967</v>
       </c>
       <c r="V21" t="n">
-        <v>0.3834</v>
+        <v>0.3854</v>
       </c>
     </row>
     <row r="22">
@@ -2052,10 +2052,10 @@
         </is>
       </c>
       <c r="U22" t="n">
-        <v>-2.3287</v>
+        <v>-2.299</v>
       </c>
       <c r="V22" t="n">
-        <v>-0.5929</v>
+        <v>-0.647</v>
       </c>
     </row>
     <row r="23">
@@ -2124,10 +2124,10 @@
         </is>
       </c>
       <c r="U23" t="n">
-        <v>0.3519</v>
+        <v>0.3518</v>
       </c>
       <c r="V23" t="n">
-        <v>-2.783</v>
+        <v>-2.795</v>
       </c>
     </row>
     <row r="24">
@@ -2196,10 +2196,10 @@
         </is>
       </c>
       <c r="U24" t="n">
-        <v>-1.1374</v>
+        <v>-1.088</v>
       </c>
       <c r="V24" t="n">
-        <v>-1.3365</v>
+        <v>-1.385</v>
       </c>
     </row>
     <row r="25">
@@ -2268,10 +2268,10 @@
         </is>
       </c>
       <c r="U25" t="n">
-        <v>-2.3298</v>
+        <v>-2.206</v>
       </c>
       <c r="V25" t="n">
-        <v>-1.045</v>
+        <v>-1.154</v>
       </c>
     </row>
     <row r="26">
@@ -2340,10 +2340,10 @@
         </is>
       </c>
       <c r="U26" t="n">
-        <v>-3.2604</v>
+        <v>-3.255</v>
       </c>
       <c r="V26" t="n">
-        <v>-1.1363</v>
+        <v>-1.148</v>
       </c>
     </row>
     <row r="27">
@@ -2412,10 +2412,10 @@
         </is>
       </c>
       <c r="U27" t="n">
-        <v>-2.8105</v>
+        <v>-2.804</v>
       </c>
       <c r="V27" t="n">
-        <v>-1.6082</v>
+        <v>-1.614</v>
       </c>
     </row>
     <row r="28">
@@ -2484,10 +2484,10 @@
         </is>
       </c>
       <c r="U28" t="n">
-        <v>0.819</v>
+        <v>0.8051</v>
       </c>
       <c r="V28" t="n">
-        <v>-3.6641</v>
+        <v>-3.639</v>
       </c>
     </row>
     <row r="29">
@@ -2556,10 +2556,10 @@
         </is>
       </c>
       <c r="U29" t="n">
-        <v>-0.3597</v>
+        <v>-0.351</v>
       </c>
       <c r="V29" t="n">
-        <v>-2.2407</v>
+        <v>-2.249</v>
       </c>
     </row>
     <row r="30">
@@ -2628,10 +2628,10 @@
         </is>
       </c>
       <c r="U30" t="n">
-        <v>0.0477</v>
+        <v>0.0589</v>
       </c>
       <c r="V30" t="n">
-        <v>-1.6698</v>
+        <v>-1.712</v>
       </c>
     </row>
     <row r="31">
@@ -2700,10 +2700,10 @@
         </is>
       </c>
       <c r="U31" t="n">
-        <v>-4.4858</v>
+        <v>-4.437</v>
       </c>
       <c r="V31" t="n">
-        <v>0.6534</v>
+        <v>0.6251</v>
       </c>
     </row>
     <row r="32">
@@ -2768,10 +2768,10 @@
         </is>
       </c>
       <c r="U32" t="n">
-        <v>-9.906599999999999</v>
+        <v>-9.926</v>
       </c>
       <c r="V32" t="n">
-        <v>-2.7599</v>
+        <v>-2.764</v>
       </c>
     </row>
     <row r="33">
@@ -2840,10 +2840,10 @@
         </is>
       </c>
       <c r="U33" t="n">
-        <v>-5.225</v>
+        <v>-5.198</v>
       </c>
       <c r="V33" t="n">
-        <v>0.1117</v>
+        <v>0.1474</v>
       </c>
     </row>
     <row r="34">
@@ -2912,10 +2912,10 @@
         </is>
       </c>
       <c r="U34" t="n">
-        <v>-6.1325</v>
+        <v>-6.12</v>
       </c>
       <c r="V34" t="n">
-        <v>0.9765</v>
+        <v>0.972</v>
       </c>
     </row>
     <row r="35">
@@ -2984,10 +2984,10 @@
         </is>
       </c>
       <c r="U35" t="n">
-        <v>-0.8943</v>
+        <v>-0.908</v>
       </c>
       <c r="V35" t="n">
-        <v>-2.5531</v>
+        <v>-2.547</v>
       </c>
     </row>
     <row r="36">
@@ -3136,10 +3136,10 @@
         </is>
       </c>
       <c r="U37" t="n">
-        <v>-4.0777</v>
+        <v>-4.084</v>
       </c>
       <c r="V37" t="n">
-        <v>-0.3366</v>
+        <v>-0.328</v>
       </c>
     </row>
     <row r="38">
@@ -3288,10 +3288,10 @@
         </is>
       </c>
       <c r="U39" t="n">
-        <v>-4.1151</v>
+        <v>-4.027</v>
       </c>
       <c r="V39" t="n">
-        <v>0.0511</v>
+        <v>0.0135</v>
       </c>
     </row>
     <row r="40">
@@ -3520,10 +3520,10 @@
         </is>
       </c>
       <c r="U42" t="n">
-        <v>-6.4878</v>
+        <v>-6.362</v>
       </c>
       <c r="V42" t="n">
-        <v>0.7272</v>
+        <v>0.6562</v>
       </c>
     </row>
     <row r="43">
@@ -3752,10 +3752,10 @@
         </is>
       </c>
       <c r="U45" t="n">
-        <v>-7.7869</v>
+        <v>-7.808</v>
       </c>
       <c r="V45" t="n">
-        <v>0.2745</v>
+        <v>0.2855</v>
       </c>
     </row>
     <row r="46">
@@ -3904,10 +3904,10 @@
         </is>
       </c>
       <c r="U47" t="n">
-        <v>-5.6172</v>
+        <v>-5.6444</v>
       </c>
       <c r="V47" t="n">
-        <v>0.5976</v>
+        <v>0.6095</v>
       </c>
     </row>
     <row r="48">
@@ -3976,10 +3976,10 @@
         </is>
       </c>
       <c r="U48" t="n">
-        <v>-3.432</v>
+        <v>-3.485</v>
       </c>
       <c r="V48" t="n">
-        <v>-5.291</v>
+        <v>-5.254</v>
       </c>
     </row>
     <row r="49">
@@ -4048,10 +4048,10 @@
         </is>
       </c>
       <c r="U49" t="n">
-        <v>-4.8686</v>
+        <v>-4.821</v>
       </c>
       <c r="V49" t="n">
-        <v>-3.4144</v>
+        <v>-3.46</v>
       </c>
     </row>
     <row r="50">
@@ -4120,10 +4120,10 @@
         </is>
       </c>
       <c r="U50" t="n">
-        <v>0.3645</v>
+        <v>0.3575</v>
       </c>
       <c r="V50" t="n">
-        <v>-6.8937</v>
+        <v>-6.892</v>
       </c>
     </row>
     <row r="51">
@@ -4272,10 +4272,10 @@
         </is>
       </c>
       <c r="U52" t="n">
-        <v>-2.5421</v>
+        <v>-2.492</v>
       </c>
       <c r="V52" t="n">
-        <v>-4.4506</v>
+        <v>-4.503</v>
       </c>
     </row>
     <row r="53">
@@ -4424,10 +4424,10 @@
         </is>
       </c>
       <c r="U54" t="n">
-        <v>-5.3988</v>
+        <v>-5.2189</v>
       </c>
       <c r="V54" t="n">
-        <v>-5.07</v>
+        <v>-5.2462</v>
       </c>
     </row>
     <row r="55">
@@ -4576,10 +4576,10 @@
         </is>
       </c>
       <c r="U56" t="n">
-        <v>-5.0479</v>
+        <v>-5.027</v>
       </c>
       <c r="V56" t="n">
-        <v>-3.0767</v>
+        <v>-3.025</v>
       </c>
     </row>
     <row r="57">
@@ -4648,10 +4648,10 @@
         </is>
       </c>
       <c r="U57" t="n">
-        <v>-3.9072</v>
+        <v>-3.923</v>
       </c>
       <c r="V57" t="n">
-        <v>-3.0008</v>
+        <v>-2.987</v>
       </c>
     </row>
     <row r="58">
@@ -5040,10 +5040,10 @@
         </is>
       </c>
       <c r="U62" t="n">
-        <v>-1.6357</v>
+        <v>-1.7</v>
       </c>
       <c r="V62" t="n">
-        <v>-1.034</v>
+        <v>-0.986</v>
       </c>
     </row>
     <row r="63">
@@ -5112,10 +5112,10 @@
         </is>
       </c>
       <c r="U63" t="n">
-        <v>0.5652</v>
+        <v>0.5228</v>
       </c>
       <c r="V63" t="n">
-        <v>-2.9832</v>
+        <v>-2.924</v>
       </c>
     </row>
     <row r="64">
@@ -5184,10 +5184,10 @@
         </is>
       </c>
       <c r="U64" t="n">
-        <v>-0.5775</v>
+        <v>-0.62</v>
       </c>
       <c r="V64" t="n">
-        <v>-1.6775</v>
+        <v>-1.626</v>
       </c>
     </row>
     <row r="65">
@@ -5256,10 +5256,10 @@
         </is>
       </c>
       <c r="U65" t="n">
-        <v>-2.4816</v>
+        <v>-2.563</v>
       </c>
       <c r="V65" t="n">
-        <v>-1.6522</v>
+        <v>-1.541</v>
       </c>
     </row>
     <row r="66">
@@ -6048,10 +6048,10 @@
         </is>
       </c>
       <c r="U75" t="n">
-        <v>-1.4196</v>
+        <v>-1.3593</v>
       </c>
       <c r="V75" t="n">
-        <v>-3.6456</v>
+        <v>-3.7091</v>
       </c>
     </row>
     <row r="76">

</xml_diff>